<commit_message>
get some plots done
</commit_message>
<xml_diff>
--- a/Literatur/Literatur.xlsx
+++ b/Literatur/Literatur.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\fvoss\Google Drive\Uni_5_Semester\Studienarbeit\Literatur\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F1B5E9B9-F58B-4B1A-BA0B-8CE4FA0708F1}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B78813BA-2330-4735-9820-DB6C6718C07E}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{93F13C59-232E-4490-8F5D-B71E96A97077}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="29" uniqueCount="20">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="22">
   <si>
     <t>Datum</t>
   </si>
@@ -94,6 +94,12 @@
   </si>
   <si>
     <t>MMR car price</t>
+  </si>
+  <si>
+    <t>Google</t>
+  </si>
+  <si>
+    <t>https://publish.manheim.com/en/help/mmr/mmr-under-the-hood.html</t>
   </si>
 </sst>
 </file>
@@ -457,7 +463,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6063F7F0-D9D7-4AF4-8A73-A83D43860DEE}">
-  <dimension ref="A1:E9"/>
+  <dimension ref="A1:E10"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="D19" sqref="D19"/>
@@ -613,18 +619,36 @@
         <v>44201</v>
       </c>
       <c r="C9" t="s">
-        <v>4</v>
+        <v>20</v>
       </c>
       <c r="D9" t="s">
         <v>19</v>
       </c>
       <c r="E9" t="s">
         <v>18</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A10">
+        <v>9</v>
+      </c>
+      <c r="B10" s="1">
+        <v>44202</v>
+      </c>
+      <c r="C10" t="s">
+        <v>20</v>
+      </c>
+      <c r="D10" t="s">
+        <v>19</v>
+      </c>
+      <c r="E10" s="2" t="s">
+        <v>21</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
     <hyperlink ref="E5" r:id="rId1" xr:uid="{D18F6FD0-0932-4D80-B7D1-78AAF16F5B9A}"/>
+    <hyperlink ref="E10" r:id="rId2" xr:uid="{0BBE904C-E281-4443-BC72-6515C95D5EBB}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Modeling start in Word Dokument
</commit_message>
<xml_diff>
--- a/Literatur/Literatur.xlsx
+++ b/Literatur/Literatur.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\fvoss\Google Drive\Uni_5_Semester\Studienarbeit\Literatur\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{682611B4-9D88-4C5F-B309-503B9B193E45}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{47003C3C-EEBD-496D-B270-14149AC9774D}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{93F13C59-232E-4490-8F5D-B71E96A97077}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="35" uniqueCount="24">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="47" uniqueCount="30">
   <si>
     <t>Datum</t>
   </si>
@@ -106,6 +106,24 @@
   </si>
   <si>
     <t>https://link.springer.com/chapter/10.1007/978-1-4419-6108-2_11</t>
+  </si>
+  <si>
+    <t>https://www.tandfonline.com/doi/pdf/10.1300/J130v05n01_02?needAccess=true</t>
+  </si>
+  <si>
+    <t>https://www.jstor.org/stable/1810022?casa_token=fVot-7ZHzHcAAAAA%3Av2RSbb-ydlHNPCWKqzpiBi9xDE178SO7x0r4brwKhlxBz2zwLNIGy6Bt1_fgrVdHRIFyyCL2CuirNEXWp7DOod2eiFDAqER6BDBPUiKnEFRxzA9vcPNR&amp;seq=1#metadata_info_tab_contents</t>
+  </si>
+  <si>
+    <t>lemon car market</t>
+  </si>
+  <si>
+    <t>George akerlof the market for lemons</t>
+  </si>
+  <si>
+    <t>https://www.williamdavid.me.uk/wp-content/uploads/2017/04/The-Market-for-Lemons-text-full.pdf</t>
+  </si>
+  <si>
+    <t>https://www.jstor.org/stable/pdf/1879431.pdf?refreqid=excelsior%3A1ff10c03269b5441b7568b90db57b572</t>
   </si>
 </sst>
 </file>
@@ -469,10 +487,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6063F7F0-D9D7-4AF4-8A73-A83D43860DEE}">
-  <dimension ref="A1:E11"/>
+  <dimension ref="A1:E15"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D12" sqref="D12"/>
+      <selection activeCell="E7" sqref="E7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -668,6 +686,74 @@
         <v>23</v>
       </c>
     </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A12">
+        <v>11</v>
+      </c>
+      <c r="B12" s="1">
+        <v>44231</v>
+      </c>
+      <c r="C12" t="s">
+        <v>4</v>
+      </c>
+      <c r="D12" t="s">
+        <v>22</v>
+      </c>
+      <c r="E12" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A13">
+        <v>12</v>
+      </c>
+      <c r="B13" s="1">
+        <v>44231</v>
+      </c>
+      <c r="C13" t="s">
+        <v>4</v>
+      </c>
+      <c r="D13" t="s">
+        <v>26</v>
+      </c>
+      <c r="E13" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A14">
+        <v>13</v>
+      </c>
+      <c r="B14" s="1">
+        <v>44231</v>
+      </c>
+      <c r="C14" t="s">
+        <v>4</v>
+      </c>
+      <c r="D14" t="s">
+        <v>27</v>
+      </c>
+      <c r="E14" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A15">
+        <v>14</v>
+      </c>
+      <c r="B15" s="1">
+        <v>44231</v>
+      </c>
+      <c r="C15" t="s">
+        <v>4</v>
+      </c>
+      <c r="D15" t="s">
+        <v>27</v>
+      </c>
+      <c r="E15" t="s">
+        <v>29</v>
+      </c>
+    </row>
   </sheetData>
   <hyperlinks>
     <hyperlink ref="E5" r:id="rId1" xr:uid="{D18F6FD0-0932-4D80-B7D1-78AAF16F5B9A}"/>

</xml_diff>